<commit_message>
power bi prototipo evaluacion
</commit_message>
<xml_diff>
--- a/Prototipo/Informacion General Cursos.xlsx
+++ b/Prototipo/Informacion General Cursos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isavi\Desktop\Universidad\PAO 2022\Tesis\Prototipo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isavi\Desktop\Universidad\PAO 2022\Tesis\PrototiposPowerBi\Prototipo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E01730-F1CE-4B4D-9FFB-4C86D8FE9C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8430551E-82B2-453C-BFCA-2A23333E58DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" activeTab="4" xr2:uid="{D1A12A75-2729-4B4C-BF6C-6F06AAF564FD}"/>
   </bookViews>
@@ -18,7 +18,8 @@
     <sheet name="modulo" sheetId="2" r:id="rId3"/>
     <sheet name="Foro" sheetId="3" r:id="rId4"/>
     <sheet name="Evaluaciones" sheetId="5" r:id="rId5"/>
-    <sheet name="Preguntas" sheetId="6" state="hidden" r:id="rId6"/>
+    <sheet name="Entregas" sheetId="7" r:id="rId6"/>
+    <sheet name="Preguntas" sheetId="6" state="hidden" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="71">
   <si>
     <t>Curso</t>
   </si>
@@ -147,15 +148,6 @@
     <t xml:space="preserve">id evaluacion </t>
   </si>
   <si>
-    <t>#nota promedio</t>
-  </si>
-  <si>
-    <t>#aprobados</t>
-  </si>
-  <si>
-    <t>#reprobado</t>
-  </si>
-  <si>
     <t>id pregunta</t>
   </si>
   <si>
@@ -208,13 +200,67 @@
   </si>
   <si>
     <t>id evaluacion</t>
+  </si>
+  <si>
+    <t>promedioAciertos</t>
+  </si>
+  <si>
+    <t>promedioFallos</t>
+  </si>
+  <si>
+    <t>Ejercicio</t>
+  </si>
+  <si>
+    <t>Correcto</t>
+  </si>
+  <si>
+    <t>Incorrecto</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Ejercicio 1</t>
+  </si>
+  <si>
+    <t>Ejercicio 2</t>
+  </si>
+  <si>
+    <t>Ejercicio 3</t>
+  </si>
+  <si>
+    <t>Ejercicio 4</t>
+  </si>
+  <si>
+    <t>Ejercicio 5</t>
+  </si>
+  <si>
+    <t>Evaluacion</t>
+  </si>
+  <si>
+    <t>Conocimientos Basicos</t>
+  </si>
+  <si>
+    <t>Introduccion</t>
+  </si>
+  <si>
+    <t>Practicas</t>
+  </si>
+  <si>
+    <t>Conocimientos Avanzados</t>
+  </si>
+  <si>
+    <t>Relacion con otras ciencias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conclusiones </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,6 +272,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -610,16 +662,16 @@
         <v>10</v>
       </c>
       <c r="H1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" t="s">
         <v>46</v>
-      </c>
-      <c r="I1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
@@ -695,7 +747,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -731,7 +783,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -792,19 +844,19 @@
         <v>33</v>
       </c>
       <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>51</v>
-      </c>
-      <c r="D1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
@@ -1573,38 +1625,40 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB030926-2EFF-4D0D-A51E-4D9916EF3D5D}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="4" max="4" width="26.07421875" customWidth="1"/>
+    <col min="5" max="5" width="16.69140625" customWidth="1"/>
+    <col min="7" max="7" width="21.69140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
@@ -1618,16 +1672,16 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>79</v>
+        <v>814</v>
       </c>
       <c r="F2">
-        <v>2000</v>
-      </c>
-      <c r="G2">
-        <v>1000</v>
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
@@ -1641,16 +1695,16 @@
         <v>3</v>
       </c>
       <c r="D3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E3">
-        <v>89</v>
+        <v>747</v>
       </c>
       <c r="F3">
-        <v>1900</v>
-      </c>
-      <c r="G3">
-        <v>1100</v>
+        <v>96</v>
+      </c>
+      <c r="G3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
@@ -1664,16 +1718,16 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E4">
+        <v>400</v>
+      </c>
+      <c r="F4">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
         <v>67</v>
-      </c>
-      <c r="F4">
-        <v>1930</v>
-      </c>
-      <c r="G4">
-        <v>1200</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
@@ -1687,24 +1741,171 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E5">
+        <v>440</v>
+      </c>
+      <c r="F5">
+        <v>84</v>
+      </c>
+      <c r="G5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>492</v>
+      </c>
+      <c r="F6">
+        <v>151</v>
+      </c>
+      <c r="G6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>649</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="G7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE10569-CE07-459B-B81E-647F071D7BC1}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
         <v>56</v>
       </c>
-      <c r="F5">
-        <v>1400</v>
-      </c>
-      <c r="G5">
-        <v>1000</v>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2">
+        <v>82</v>
+      </c>
+      <c r="C2">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <v>91</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4">
+        <v>85</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5">
+        <v>92</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <v>60</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5434A0D-079C-4E93-8AFD-BE9804A83C72}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -1716,16 +1917,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>